<commit_message>
Updated demo application and LCA data with less impacful hardening process.
</commit_message>
<xml_diff>
--- a/public/lcad-evaluation/assets/data/LCA/Design A/Impact Assessment A - GWP.XLSX
+++ b/public/lcad-evaluation/assets/data/LCA/Design A/Impact Assessment A - GWP.XLSX
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="XLSReadWriteII" lastEdited="4" lowestEdited="4" rupBuild="4.00.38"/>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet5" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -51,9 +51,6 @@
     <t>Sort order: </t>
   </si>
   <si>
-    <t>Induction Hardening Bearing Surface 1</t>
-  </si>
-  <si>
     <t>Analyze</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Turning Chamfer 6</t>
+  </si>
+  <si>
+    <t>Induction Hardening Bearing Surfaces 1, 2</t>
   </si>
   <si>
     <t>Total</t>
@@ -521,24 +521,24 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="1">
-        <v>45571</v>
+        <v>45572</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="2">
-        <v>0.577786898148148</v>
+        <v>0.809568472222222</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
@@ -549,15 +549,15 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -586,7 +586,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -629,25 +629,25 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
         <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" t="s">
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I16" t="s">
         <v>36</v>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="Q16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R16" t="s">
         <v>44</v>
@@ -683,13 +683,13 @@
         <v>35</v>
       </c>
       <c r="T16" t="s">
+        <v>24</v>
+      </c>
+      <c r="U16" t="s">
+        <v>14</v>
+      </c>
+      <c r="V16" t="s">
         <v>25</v>
-      </c>
-      <c r="U16" t="s">
-        <v>15</v>
-      </c>
-      <c r="V16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -700,7 +700,7 @@
         <v>34</v>
       </c>
       <c r="C17">
-        <v>212.631321243125</v>
+        <v>173.688803990365</v>
       </c>
       <c r="D17">
         <v>63.9589323653056</v>
@@ -757,7 +757,7 @@
         <v>0.00859644008161318</v>
       </c>
       <c r="V17">
-        <v>73.0172198489251</v>
+        <v>34.074702596165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>